<commit_message>
extend for a combined sample analysis and plots
</commit_message>
<xml_diff>
--- a/data/scenario_parameters.xlsx
+++ b/data/scenario_parameters.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngreen1\Google Drive\ACE -- LTBI screening in hospital\R code\LTBIhospitalScreenACE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120C0188-4BAF-4F4E-BB1D-1C949401E0C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,23 +16,17 @@
     <sheet name="p" sheetId="1" r:id="rId1"/>
     <sheet name="cost" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
-  <si>
-    <t>Agree to Screen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="12">
   <si>
     <t>Sensitivity</t>
   </si>
   <si>
     <t>Specificity</t>
-  </si>
-  <si>
-    <t>Not Agree to Screen</t>
   </si>
   <si>
     <t>scenario</t>
@@ -49,13 +44,19 @@
     <t>distn</t>
   </si>
   <si>
-    <t>unif</t>
-  </si>
-  <si>
     <t>1-Sensitivity</t>
   </si>
   <si>
     <t>1-Specificity</t>
+  </si>
+  <si>
+    <t>LTBI</t>
+  </si>
+  <si>
+    <t>non-LTBI</t>
+  </si>
+  <si>
+    <t>unif</t>
   </si>
 </sst>
 </file>
@@ -407,18 +408,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -426,39 +425,40 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="B2">
+        <f>1-A2</f>
+        <v>0.8</v>
+      </c>
+      <c r="C2">
         <v>0.84</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.99</v>
-      </c>
-      <c r="D2">
-        <v>0.4</v>
       </c>
       <c r="E2">
         <v>0.16000000000000003</v>
@@ -472,16 +472,17 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">1-A3</f>
+        <v>0.7</v>
+      </c>
+      <c r="C3">
         <v>0.84</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.99</v>
-      </c>
-      <c r="D3">
-        <v>0.4</v>
       </c>
       <c r="E3">
         <v>0.16000000000000003</v>
@@ -491,6 +492,174 @@
       </c>
       <c r="G3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.4</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="C4">
+        <v>0.84</v>
+      </c>
+      <c r="D4">
+        <v>0.99</v>
+      </c>
+      <c r="E4">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F4">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.2</v>
+      </c>
+      <c r="B5">
+        <f>1-A5</f>
+        <v>0.8</v>
+      </c>
+      <c r="C5">
+        <v>0.84</v>
+      </c>
+      <c r="D5">
+        <v>0.99</v>
+      </c>
+      <c r="E5">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F5">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.3</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B7" si="1">1-A6</f>
+        <v>0.7</v>
+      </c>
+      <c r="C6">
+        <v>0.84</v>
+      </c>
+      <c r="D6">
+        <v>0.99</v>
+      </c>
+      <c r="E6">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F6">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="C7">
+        <v>0.84</v>
+      </c>
+      <c r="D7">
+        <v>0.99</v>
+      </c>
+      <c r="E7">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F7">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.2</v>
+      </c>
+      <c r="B8">
+        <f>1-A8</f>
+        <v>0.8</v>
+      </c>
+      <c r="C8">
+        <v>0.84</v>
+      </c>
+      <c r="D8">
+        <v>0.99</v>
+      </c>
+      <c r="E8">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F8">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B10" si="2">1-A9</f>
+        <v>0.7</v>
+      </c>
+      <c r="C9">
+        <v>0.84</v>
+      </c>
+      <c r="D9">
+        <v>0.99</v>
+      </c>
+      <c r="E9">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F9">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="C10">
+        <v>0.84</v>
+      </c>
+      <c r="D10">
+        <v>0.99</v>
+      </c>
+      <c r="E10">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F10">
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -500,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,19 +682,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,13 +702,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -547,19 +716,597 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>144</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>144</v>
+      </c>
+      <c r="C4">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>144</v>
+      </c>
+      <c r="C5">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B6">
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>144</v>
+      </c>
+      <c r="C7">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <v>144</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>144</v>
+      </c>
+      <c r="C9">
+        <v>144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>144</v>
+      </c>
+      <c r="C10">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>144</v>
+      </c>
+      <c r="C11">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>144</v>
+      </c>
+      <c r="C12">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>144</v>
+      </c>
+      <c r="C13">
+        <v>144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>147</v>
+      </c>
+      <c r="C14">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>147</v>
+      </c>
+      <c r="C15">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>147</v>
+      </c>
+      <c r="C16">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>147</v>
+      </c>
+      <c r="C17">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>147</v>
+      </c>
+      <c r="C18">
+        <v>147</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>147</v>
+      </c>
+      <c r="C19">
+        <v>147</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>147</v>
+      </c>
+      <c r="C20">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>147</v>
+      </c>
+      <c r="C21">
+        <v>147</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>147</v>
+      </c>
+      <c r="C22">
+        <v>147</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>147</v>
+      </c>
+      <c r="C23">
+        <v>147</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>147</v>
+      </c>
+      <c r="C24">
+        <v>147</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>147</v>
+      </c>
+      <c r="C25">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>146</v>
+      </c>
+      <c r="C26">
+        <v>146</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>146</v>
+      </c>
+      <c r="C27">
+        <v>146</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>146</v>
+      </c>
+      <c r="C28">
+        <v>146</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>146</v>
+      </c>
+      <c r="C29">
+        <v>146</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>146</v>
+      </c>
+      <c r="C30">
+        <v>146</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>146</v>
+      </c>
+      <c r="C31">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>146</v>
+      </c>
+      <c r="C32">
+        <v>146</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>146</v>
+      </c>
+      <c r="C33">
+        <v>146</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>146</v>
+      </c>
+      <c r="C34">
+        <v>146</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>146</v>
+      </c>
+      <c r="C35">
+        <v>146</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>146</v>
+      </c>
+      <c r="C36">
+        <v>146</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>146</v>
+      </c>
+      <c r="C37">
+        <v>146</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more small changes for GP decision tree
</commit_message>
<xml_diff>
--- a/data/scenario_parameters.xlsx
+++ b/data/scenario_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngreen1\Google Drive\ACE -- LTBI screening in hospital\R code\LTBIhospitalScreenACE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120C0188-4BAF-4F4E-BB1D-1C949401E0C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27E54F6-A821-464F-A8D3-D9EC31091960}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="13">
   <si>
     <t>Sensitivity</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>unif</t>
+  </si>
+  <si>
+    <t>Not Agree to Screen</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -669,10 +672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,24 +770,26 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>144</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="C6">
-        <v>144</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>144</v>
@@ -801,7 +806,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>144</v>
@@ -818,7 +823,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>144</v>
@@ -835,7 +840,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>144</v>
@@ -847,29 +852,31 @@
         <v>11</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>144</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="C11">
-        <v>144</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B12">
         <v>144</v>
@@ -886,7 +893,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>144</v>
@@ -903,58 +910,60 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C14">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C15">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>147</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="C16">
-        <v>147</v>
+        <f>144-12-5.96</f>
+        <v>126.04</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B17">
         <v>147</v>
@@ -971,7 +980,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>147</v>
@@ -983,12 +992,12 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>147</v>
@@ -1000,12 +1009,12 @@
         <v>11</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>147</v>
@@ -1017,24 +1026,26 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>147</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="C21">
-        <v>147</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1051,7 +1062,7 @@
         <v>11</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,7 +1079,7 @@
         <v>11</v>
       </c>
       <c r="E23">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="E24">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,114 +1113,118 @@
         <v>11</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B26">
-        <v>146</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="C26">
-        <v>146</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C27">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C28">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C30">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B31">
-        <v>146</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="C31">
-        <v>146</v>
+        <f>147-12-5.96</f>
+        <v>129.04</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>146</v>
@@ -1221,12 +1236,12 @@
         <v>11</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>146</v>
@@ -1238,12 +1253,12 @@
         <v>11</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B34">
         <v>146</v>
@@ -1255,12 +1270,12 @@
         <v>11</v>
       </c>
       <c r="E34">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>146</v>
@@ -1272,29 +1287,31 @@
         <v>11</v>
       </c>
       <c r="E35">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B36">
-        <v>146</v>
+        <f>146-12-5.96</f>
+        <v>128.04</v>
       </c>
       <c r="C36">
-        <v>146</v>
+        <f>146-12-5.96</f>
+        <v>128.04</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>146</v>
@@ -1306,6 +1323,163 @@
         <v>11</v>
       </c>
       <c r="E37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>146</v>
+      </c>
+      <c r="C38">
+        <v>146</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39">
+        <v>146</v>
+      </c>
+      <c r="C39">
+        <v>146</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>146</v>
+      </c>
+      <c r="C40">
+        <v>146</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <f>146-12-5.96</f>
+        <v>128.04</v>
+      </c>
+      <c r="C41">
+        <f>146-12-5.96</f>
+        <v>128.04</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>146</v>
+      </c>
+      <c r="C42">
+        <v>146</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>146</v>
+      </c>
+      <c r="C43">
+        <v>146</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>146</v>
+      </c>
+      <c r="C44">
+        <v>146</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>146</v>
+      </c>
+      <c r="C45">
+        <v>146</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <f>146-12-5.96</f>
+        <v>128.04</v>
+      </c>
+      <c r="C46">
+        <f>146-12-5.96</f>
+        <v>128.04</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
         <v>9</v>
       </c>
     </row>

</xml_diff>